<commit_message>
Calcolo area e perimetro del rettangolo
</commit_message>
<xml_diff>
--- a/Excel/Area e perimetro rettangolo.xlsx
+++ b/Excel/Area e perimetro rettangolo.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/OneDrive/Scuola/Flowchart/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/Sviluppo/Didattica/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73C21C0-B0ED-7544-847B-4F1B3DE0D627}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +17,7 @@
     <sheet name="Controllo input" sheetId="1" r:id="rId2"/>
     <sheet name="Controllo input avanzato" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -149,22 +150,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -482,125 +483,126 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
         <f>A4*B4</f>
         <v>2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>(A4+B4)*2</f>
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" ref="D5:D8" si="0">A5*B5</f>
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" ref="E5:E8" si="1">(A5+B5)*2</f>
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
         <v>-2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>-1</v>
       </c>
-      <c r="B7" s="7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>-1</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>-2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="1"/>
         <v>-6</v>
       </c>
@@ -612,6 +614,7 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -629,116 +632,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
         <f>IF(AND(A4&gt;0,B4&gt;0),A4*B4,"ERRORE MISURE LATI")</f>
         <v>2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>IF(AND(A4&gt;0,B4&gt;0),(A4+B4)*2,"ERRORE MISURE LATI")</f>
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" ref="D5:D8" si="0">IF(AND(A5&gt;0,B5&gt;0),A5*B5,"ERRORE MISURE LATI")</f>
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" ref="E5:E8" si="1">IF(AND(A5&gt;0,B5&gt;0),(A5+B5)*2,"ERRORE MISURE LATI")</f>
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
         <v>-2</v>
       </c>
-      <c r="D6" s="3" t="str">
+      <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ERRORE MISURE LATI</v>
       </c>
-      <c r="E6" s="3" t="str">
+      <c r="E6" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ERRORE MISURE LATI</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>-1</v>
       </c>
-      <c r="B7" s="7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="str">
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ERRORE MISURE LATI</v>
       </c>
-      <c r="E7" s="3" t="str">
+      <c r="E7" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ERRORE MISURE LATI</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>-1</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>-2</v>
       </c>
-      <c r="D8" s="11" t="str">
+      <c r="D8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>ERRORE MISURE LATI</v>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E8" s="8" t="str">
         <f t="shared" si="1"/>
         <v>ERRORE MISURE LATI</v>
       </c>
@@ -759,7 +762,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -769,116 +772,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
         <f>IF(A4&gt;0,IF(B4&gt;0,A4*B4,"MISURA LATO 2 ERRATA"),"MISURA LATO 1 ERRATA")</f>
         <v>2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>IF(A4&gt;0,IF(B4&gt;0,(A4+B4)*2,"MISURA LATO 2 ERRATA"),"MISURA LATO 1 ERRATA")</f>
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" ref="D5:D8" si="0">IF(A5&gt;0,IF(B5&gt;0,A5*B5,"MISURA LATO 2 ERRATA"),"MISURA LATO 1 ERRATA")</f>
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f>IF(A5&gt;0,IF(B5&gt;0,(A5+B5)*2,"MISURA LATO 2 ERRATA"),"MISURA LATO 1 ERRATA")</f>
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
         <v>-2</v>
       </c>
-      <c r="D6" s="3" t="str">
+      <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MISURA LATO 2 ERRATA</v>
       </c>
-      <c r="E6" s="3" t="str">
+      <c r="E6" s="2" t="str">
         <f>IF(A6&gt;0,IF(B6&gt;0,(A6+B6)*2,"MISURA LATO 2 ERRATA"),"MISURA LATO 1 ERRATA")</f>
         <v>MISURA LATO 2 ERRATA</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>-1</v>
       </c>
-      <c r="B7" s="7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="str">
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MISURA LATO 1 ERRATA</v>
       </c>
-      <c r="E7" s="3" t="str">
+      <c r="E7" s="2" t="str">
         <f>IF(A7&gt;0,IF(B7&gt;0,(A7+B7)*2,"MISURA LATO 2 ERRATA"),"MISURA LATO 1 ERRATA")</f>
         <v>MISURA LATO 1 ERRATA</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>-1</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>-2</v>
       </c>
-      <c r="D8" s="3" t="str">
+      <c r="D8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MISURA LATO 1 ERRATA</v>
       </c>
-      <c r="E8" s="3" t="str">
+      <c r="E8" s="2" t="str">
         <f>IF(A8&gt;0,IF(B8&gt;0,(A8+B8)*2,"MISURA LATO 2 ERRATA"),"MISURA LATO 1 ERRATA")</f>
         <v>MISURA LATO 1 ERRATA</v>
       </c>

</xml_diff>